<commit_message>
Custom Sort and Original Sort/Unsort
</commit_message>
<xml_diff>
--- a/Microsoft_Excel_by_Leila_Gharani.xlsx
+++ b/Microsoft_Excel_by_Leila_Gharani.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iNeuron\Microsoft_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC85D57-8E2F-4F17-8A18-67A4033623CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518C54F9-2297-4D32-B596-25DF861631C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day-1" sheetId="1" r:id="rId1"/>
     <sheet name="Day-2" sheetId="2" r:id="rId2"/>
     <sheet name="Day-3" sheetId="3" r:id="rId3"/>
+    <sheet name="Day-4" sheetId="4" r:id="rId4"/>
+    <sheet name="Day-5" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Day-2'!$C$3:$F$29</definedName>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="57">
   <si>
     <t>Absolute, Relative and Mixed Cell Referencing</t>
   </si>
@@ -181,12 +183,87 @@
   <si>
     <t>&lt;400</t>
   </si>
+  <si>
+    <t>Excel Sort Basics</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Apps</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Utility</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>Accord</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Misty Wash</t>
+  </si>
+  <si>
+    <t>Productivity</t>
+  </si>
+  <si>
+    <t>WenCaL</t>
+  </si>
+  <si>
+    <t>Sleops</t>
+  </si>
+  <si>
+    <t>Blend</t>
+  </si>
+  <si>
+    <t>Twenty20</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>South America</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>Hackrr</t>
+  </si>
+  <si>
+    <t>Fightrr</t>
+  </si>
+  <si>
+    <t>Kryptis</t>
+  </si>
+  <si>
+    <t>Perino</t>
+  </si>
+  <si>
+    <t>Sort/Unsort</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +321,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Schriftart für Textkörper"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -265,7 +357,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -393,13 +485,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -439,17 +542,29 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{DA3F0C31-CC79-4E87-AFB1-7A6099006D56}"/>
+    <cellStyle name="Hyperlink 3" xfId="4" xr:uid="{C4CE5DF7-4AB3-4E3B-B8AF-6BB298E76A64}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{27E0D15E-1D11-4E0E-9819-2BF1029C6403}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
@@ -460,26 +575,32 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right/>
         <top/>
         <bottom/>
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -492,6 +613,65 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
@@ -499,6 +679,56 @@
         </right>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -539,121 +769,6 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -938,12 +1053,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E02ABB8D-9743-4B7E-B6EA-A02BD272C64C}" name="Table2" displayName="Table2" ref="D3:G30" totalsRowCount="1" headerRowDxfId="4" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E02ABB8D-9743-4B7E-B6EA-A02BD272C64C}" name="Table2" displayName="Table2" ref="D3:G30" totalsRowCount="1" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7D149612-333D-4F8F-A7D3-CE7875BF0A5F}" name="Channel" totalsRowLabel="Total" dataDxfId="8" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{EB3B883E-008D-47A2-B372-FEBA8A25D63F}" name="Product" totalsRowFunction="count" dataDxfId="7" totalsRowDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{08805D3D-07B4-4FFF-BFE2-C02148D098E9}" name="Date" dataDxfId="6" totalsRowDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{ED916B00-D255-4E2D-94B3-9BD17081553B}" name="Sales Value" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{7D149612-333D-4F8F-A7D3-CE7875BF0A5F}" name="Channel" totalsRowLabel="Total" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{EB3B883E-008D-47A2-B372-FEBA8A25D63F}" name="Product" totalsRowFunction="count" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{08805D3D-07B4-4FFF-BFE2-C02148D098E9}" name="Date" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{ED916B00-D255-4E2D-94B3-9BD17081553B}" name="Sales Value" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1218,22 +1333,22 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:13" ht="15" thickBot="1">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>1</v>
@@ -1267,7 +1382,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -1311,7 +1426,7 @@
         <v>0.27272727272727271</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
@@ -1355,7 +1470,7 @@
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -1399,7 +1514,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13">
       <c r="F7" s="2">
         <f>SUM(F4:F6)</f>
         <v>2495</v>
@@ -1409,17 +1524,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1441,7 +1556,7 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
@@ -1449,16 +1564,16 @@
     <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1">
+      <c r="A1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="31"/>
       <c r="D1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="C3" s="12" t="s">
         <v>14</v>
       </c>
@@ -1472,7 +1587,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="C4" s="11" t="s">
         <v>18</v>
       </c>
@@ -1486,7 +1601,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="C5" s="11" t="s">
         <v>20</v>
       </c>
@@ -1500,7 +1615,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="C6" s="11" t="s">
         <v>22</v>
       </c>
@@ -1514,7 +1629,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="C7" s="11" t="s">
         <v>20</v>
       </c>
@@ -1528,7 +1643,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="C8" s="11" t="s">
         <v>22</v>
       </c>
@@ -1542,7 +1657,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="C9" s="11" t="s">
         <v>18</v>
       </c>
@@ -1556,7 +1671,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="C10" s="11" t="s">
         <v>20</v>
       </c>
@@ -1570,7 +1685,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="C11" s="11" t="s">
         <v>20</v>
       </c>
@@ -1584,7 +1699,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="C12" s="11" t="s">
         <v>18</v>
       </c>
@@ -1598,7 +1713,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="C13" s="11" t="s">
         <v>20</v>
       </c>
@@ -1612,7 +1727,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6">
       <c r="C14" s="11" t="s">
         <v>22</v>
       </c>
@@ -1626,7 +1741,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="C15" s="11" t="s">
         <v>20</v>
       </c>
@@ -1640,7 +1755,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6">
       <c r="C16" s="11" t="s">
         <v>20</v>
       </c>
@@ -1654,7 +1769,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6">
       <c r="C17" s="11" t="s">
         <v>22</v>
       </c>
@@ -1668,7 +1783,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:6">
       <c r="C18" s="11" t="s">
         <v>20</v>
       </c>
@@ -1682,7 +1797,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:6">
       <c r="C19" s="11" t="s">
         <v>22</v>
       </c>
@@ -1696,7 +1811,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:6">
       <c r="C20" s="11" t="s">
         <v>20</v>
       </c>
@@ -1710,7 +1825,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:6">
       <c r="C21" s="11" t="s">
         <v>20</v>
       </c>
@@ -1724,7 +1839,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:6">
       <c r="C22" s="11" t="s">
         <v>22</v>
       </c>
@@ -1738,7 +1853,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:6">
       <c r="C23" s="11" t="s">
         <v>20</v>
       </c>
@@ -1752,7 +1867,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:6">
       <c r="C24" s="11" t="s">
         <v>20</v>
       </c>
@@ -1766,7 +1881,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:6">
       <c r="C25" s="11" t="s">
         <v>20</v>
       </c>
@@ -1780,7 +1895,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:6">
       <c r="C26" s="11" t="s">
         <v>22</v>
       </c>
@@ -1794,7 +1909,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:6">
       <c r="C27" s="11" t="s">
         <v>20</v>
       </c>
@@ -1808,7 +1923,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:6">
       <c r="C28" s="11" t="s">
         <v>20</v>
       </c>
@@ -1822,7 +1937,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:6">
       <c r="C29" s="15" t="s">
         <v>22</v>
       </c>
@@ -1836,7 +1951,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:6">
       <c r="C30" s="18" t="s">
         <v>8</v>
       </c>
@@ -1865,11 +1980,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD893A58-35C4-4ADC-96F1-E62CA20E0C55}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
@@ -1879,26 +1994,26 @@
     <col min="10" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:12" ht="15" thickBot="1">
+      <c r="A1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="I1" s="31" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="I1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12">
       <c r="I2" s="9" t="s">
         <v>20</v>
       </c>
@@ -1912,17 +2027,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D3" s="27" t="s">
+    <row r="3" spans="1:12">
+      <c r="D3" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="28" t="s">
         <v>17</v>
       </c>
       <c r="I3" s="9" t="s">
@@ -1938,7 +2053,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12">
       <c r="D4" s="11" t="s">
         <v>18</v>
       </c>
@@ -1948,11 +2063,11 @@
       <c r="F4" s="10">
         <v>43108</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="29">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="D5" s="11" t="s">
         <v>20</v>
       </c>
@@ -1962,14 +2077,14 @@
       <c r="F5" s="10">
         <v>43108</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="29">
         <v>250</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="27" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12">
       <c r="D6" s="11" t="s">
         <v>22</v>
       </c>
@@ -1979,14 +2094,14 @@
       <c r="F6" s="10">
         <v>43111</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="29">
         <v>300</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12">
       <c r="D7" s="11" t="s">
         <v>20</v>
       </c>
@@ -1996,14 +2111,14 @@
       <c r="F7" s="10">
         <v>43141</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="29">
         <v>260</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12">
       <c r="D8" s="11" t="s">
         <v>22</v>
       </c>
@@ -2013,14 +2128,14 @@
       <c r="F8" s="10">
         <v>43141</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8" s="29">
         <v>270</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="D9" s="11" t="s">
         <v>18</v>
       </c>
@@ -2030,14 +2145,14 @@
       <c r="F9" s="10">
         <v>43089</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9" s="29">
         <v>280</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12">
       <c r="D10" s="11" t="s">
         <v>20</v>
       </c>
@@ -2047,14 +2162,14 @@
       <c r="F10" s="10">
         <v>43040</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="29">
         <v>100</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12">
       <c r="D11" s="11" t="s">
         <v>20</v>
       </c>
@@ -2064,11 +2179,11 @@
       <c r="F11" s="10">
         <v>43040</v>
       </c>
-      <c r="G11" s="30">
+      <c r="G11" s="29">
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12">
       <c r="D12" s="11" t="s">
         <v>18</v>
       </c>
@@ -2078,11 +2193,11 @@
       <c r="F12" s="10">
         <v>43040</v>
       </c>
-      <c r="G12" s="30">
+      <c r="G12" s="29">
         <v>410</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12">
       <c r="D13" s="11" t="s">
         <v>20</v>
       </c>
@@ -2092,11 +2207,11 @@
       <c r="F13" s="10">
         <v>43089</v>
       </c>
-      <c r="G13" s="30">
+      <c r="G13" s="29">
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12">
       <c r="D14" s="11" t="s">
         <v>22</v>
       </c>
@@ -2106,11 +2221,11 @@
       <c r="F14" s="10">
         <v>43089</v>
       </c>
-      <c r="G14" s="30">
+      <c r="G14" s="29">
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12">
       <c r="D15" s="11" t="s">
         <v>20</v>
       </c>
@@ -2120,11 +2235,11 @@
       <c r="F15" s="10">
         <v>43089</v>
       </c>
-      <c r="G15" s="30">
+      <c r="G15" s="29">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12">
       <c r="D16" s="11" t="s">
         <v>20</v>
       </c>
@@ -2134,11 +2249,11 @@
       <c r="F16" s="10">
         <v>43108</v>
       </c>
-      <c r="G16" s="30">
+      <c r="G16" s="29">
         <v>401</v>
       </c>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:7">
       <c r="D17" s="11" t="s">
         <v>22</v>
       </c>
@@ -2148,11 +2263,11 @@
       <c r="F17" s="10">
         <v>43108</v>
       </c>
-      <c r="G17" s="30">
+      <c r="G17" s="29">
         <v>430</v>
       </c>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:7">
       <c r="D18" s="11" t="s">
         <v>20</v>
       </c>
@@ -2162,11 +2277,11 @@
       <c r="F18" s="10">
         <v>43108</v>
       </c>
-      <c r="G18" s="30">
+      <c r="G18" s="29">
         <v>285</v>
       </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:7">
       <c r="D19" s="11" t="s">
         <v>22</v>
       </c>
@@ -2176,11 +2291,11 @@
       <c r="F19" s="10">
         <v>43111</v>
       </c>
-      <c r="G19" s="30">
+      <c r="G19" s="29">
         <v>344</v>
       </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:7">
       <c r="D20" s="11" t="s">
         <v>20</v>
       </c>
@@ -2190,11 +2305,11 @@
       <c r="F20" s="10">
         <v>43141</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="29">
         <v>304</v>
       </c>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:7">
       <c r="D21" s="11" t="s">
         <v>20</v>
       </c>
@@ -2204,11 +2319,11 @@
       <c r="F21" s="10">
         <v>43110</v>
       </c>
-      <c r="G21" s="30">
+      <c r="G21" s="29">
         <v>431</v>
       </c>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:7">
       <c r="D22" s="11" t="s">
         <v>22</v>
       </c>
@@ -2218,11 +2333,11 @@
       <c r="F22" s="10">
         <v>43110</v>
       </c>
-      <c r="G22" s="30">
+      <c r="G22" s="29">
         <v>298</v>
       </c>
     </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:7">
       <c r="D23" s="11" t="s">
         <v>20</v>
       </c>
@@ -2232,11 +2347,11 @@
       <c r="F23" s="10">
         <v>43110</v>
       </c>
-      <c r="G23" s="30">
+      <c r="G23" s="29">
         <v>258</v>
       </c>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:7">
       <c r="D24" s="11" t="s">
         <v>20</v>
       </c>
@@ -2246,11 +2361,11 @@
       <c r="F24" s="10">
         <v>43110</v>
       </c>
-      <c r="G24" s="30">
+      <c r="G24" s="29">
         <v>251</v>
       </c>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:7">
       <c r="D25" s="11" t="s">
         <v>20</v>
       </c>
@@ -2260,11 +2375,11 @@
       <c r="F25" s="10">
         <v>43079</v>
       </c>
-      <c r="G25" s="30">
+      <c r="G25" s="29">
         <v>260</v>
       </c>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:7">
       <c r="D26" s="11" t="s">
         <v>22</v>
       </c>
@@ -2274,11 +2389,11 @@
       <c r="F26" s="10">
         <v>43079</v>
       </c>
-      <c r="G26" s="30">
+      <c r="G26" s="29">
         <v>415</v>
       </c>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:7">
       <c r="D27" s="11" t="s">
         <v>20</v>
       </c>
@@ -2288,11 +2403,11 @@
       <c r="F27" s="10">
         <v>43049</v>
       </c>
-      <c r="G27" s="30">
+      <c r="G27" s="29">
         <v>266</v>
       </c>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:7">
       <c r="D28" s="11" t="s">
         <v>20</v>
       </c>
@@ -2302,11 +2417,11 @@
       <c r="F28" s="10">
         <v>43049</v>
       </c>
-      <c r="G28" s="30">
+      <c r="G28" s="29">
         <v>425</v>
       </c>
     </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:7">
       <c r="D29" s="15" t="s">
         <v>22</v>
       </c>
@@ -2316,11 +2431,11 @@
       <c r="F29" s="17">
         <v>43108</v>
       </c>
-      <c r="G29" s="26">
+      <c r="G29" s="25">
         <v>429</v>
       </c>
     </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:7">
       <c r="D30" s="15" t="s">
         <v>8</v>
       </c>
@@ -2329,7 +2444,7 @@
         <v>26</v>
       </c>
       <c r="F30" s="16"/>
-      <c r="G30" s="26">
+      <c r="G30" s="25">
         <f>SUBTOTAL(109,Table2[Sales Value])</f>
         <v>8167</v>
       </c>
@@ -2343,4 +2458,1168 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BDF7D00-80FC-42C0-A490-F9016C3DF4B0}">
+  <dimension ref="A1:F38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1">
+      <c r="A1" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="31"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="C4" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="C5" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="34">
+        <v>47296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="C6" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="34">
+        <v>8132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="C7" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="34">
+        <v>6487</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="C8" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="34">
+        <v>29277</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="C9" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="34">
+        <v>26412</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="C10" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="34">
+        <v>8532</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="C11" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="34">
+        <v>49988</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="C12" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="34">
+        <v>49144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="C13" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="34">
+        <v>34155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="C14" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="34">
+        <v>46652</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="C15" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="34">
+        <v>28020</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="C16" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="34">
+        <v>28523</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6">
+      <c r="C17" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="34">
+        <v>90530</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="C18" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="34">
+        <v>46994</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6">
+      <c r="C19" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="34">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="C20" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="34">
+        <v>34196</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6">
+      <c r="C21" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="34">
+        <v>85200</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6">
+      <c r="C22" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="34">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6">
+      <c r="C23" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="34">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6">
+      <c r="C24" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="34">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6">
+      <c r="C25" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="34">
+        <v>20898</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6">
+      <c r="C26" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="34">
+        <v>43784</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6">
+      <c r="C27" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="34">
+        <v>34155</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6">
+      <c r="C28" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="34">
+        <v>19789</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6">
+      <c r="C29" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" s="34">
+        <v>49656</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6">
+      <c r="C30" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="34">
+        <v>9432</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6">
+      <c r="C31" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" s="34">
+        <v>46922</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6">
+      <c r="C32" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="34">
+        <v>46336</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6">
+      <c r="C33" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" s="34">
+        <v>30832</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6">
+      <c r="C34" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" s="34">
+        <v>44675</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6">
+      <c r="C35" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="34">
+        <v>13596</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6">
+      <c r="C36" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="F36" s="34">
+        <v>42569</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6">
+      <c r="C37" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F37" s="34">
+        <v>18524</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6">
+      <c r="C38" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" s="34">
+        <v>2116</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C5:F38">
+    <sortCondition ref="C5:C38" customList="Productivity,Utility,Game"/>
+    <sortCondition ref="D5:D38"/>
+    <sortCondition sortBy="icon" ref="F5:F38" iconSet="3Flags" iconId="2"/>
+    <sortCondition sortBy="icon" ref="F5:F38" iconSet="3Flags" iconId="1"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F5:F38">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Flags">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADED6C27-6C18-4AA2-A056-D97167A8B3BE}">
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1">
+      <c r="A1" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="31"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="37">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5" s="35">
+        <v>2</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="37">
+        <v>46994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="C6" s="35">
+        <v>3</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="37">
+        <v>34155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7" s="35">
+        <v>4</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="37">
+        <v>49144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="C8" s="35">
+        <v>5</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="37">
+        <v>49988</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="C9" s="35">
+        <v>6</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="37">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="C10" s="35">
+        <v>7</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="37">
+        <v>90530</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="C11" s="35">
+        <v>8</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="37">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="C12" s="35">
+        <v>9</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="37">
+        <v>34196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="C13" s="35">
+        <v>10</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="37">
+        <v>46652</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="C14" s="35">
+        <v>11</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="37">
+        <v>28523</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="C15" s="35">
+        <v>12</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="37">
+        <v>20898</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="C16" s="35">
+        <v>13</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="37">
+        <v>8132</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7">
+      <c r="C17" s="35">
+        <v>14</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="37">
+        <v>47296</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7">
+      <c r="C18" s="35">
+        <v>15</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="37">
+        <v>8532</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7">
+      <c r="C19" s="35">
+        <v>16</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="37">
+        <v>44675</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7">
+      <c r="C20" s="35">
+        <v>17</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="37">
+        <v>42569</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7">
+      <c r="C21" s="35">
+        <v>18</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="37">
+        <v>18524</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7">
+      <c r="C22" s="35">
+        <v>19</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="37">
+        <v>2116</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7">
+      <c r="C23" s="35">
+        <v>20</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="37">
+        <v>13596</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7">
+      <c r="C24" s="35">
+        <v>21</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="37">
+        <v>6487</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7">
+      <c r="C25" s="35">
+        <v>22</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="37">
+        <v>26412</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7">
+      <c r="C26" s="35">
+        <v>23</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="37">
+        <v>29277</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7">
+      <c r="C27" s="35">
+        <v>24</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="G27" s="37">
+        <v>34155</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7">
+      <c r="C28" s="35">
+        <v>25</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="37">
+        <v>19789</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7">
+      <c r="C29" s="35">
+        <v>26</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="37">
+        <v>43784</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7">
+      <c r="C30" s="35">
+        <v>27</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" s="37">
+        <v>28020</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7">
+      <c r="C31" s="35">
+        <v>28</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="37">
+        <v>46336</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7">
+      <c r="C32" s="35">
+        <v>29</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="37">
+        <v>30832</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7">
+      <c r="C33" s="35">
+        <v>30</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" s="37">
+        <v>85200</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7">
+      <c r="C34" s="35">
+        <v>31</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="37">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7">
+      <c r="C35" s="35">
+        <v>32</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="G35" s="37">
+        <v>46922</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7">
+      <c r="C36" s="35">
+        <v>33</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G36" s="37">
+        <v>49656</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7">
+      <c r="C37" s="35">
+        <v>34</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="G37" s="37">
+        <v>9432</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C4:G37">
+    <sortCondition ref="C4:C37"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Calculate % in excel the right way
</commit_message>
<xml_diff>
--- a/Microsoft_Excel_by_Leila_Gharani.xlsx
+++ b/Microsoft_Excel_by_Leila_Gharani.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iNeuron\Microsoft_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7F448B-57AA-4A9C-8C55-6850D8940C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5BEEA6-2A43-4891-B1FD-5DE9C3ED6B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day-1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Day-6" sheetId="6" r:id="rId6"/>
     <sheet name="Day-7" sheetId="7" r:id="rId7"/>
     <sheet name="Day-8" sheetId="10" r:id="rId8"/>
+    <sheet name="Day-9" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Day-2'!$C$3:$F$29</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="137">
   <si>
     <t>Absolute, Relative and Mixed Cell Referencing</t>
   </si>
@@ -408,12 +409,108 @@
   <si>
     <t>Headers &amp; Footers</t>
   </si>
+  <si>
+    <t>Calculate Percentage in Excel the right way!</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Sophia</t>
+  </si>
+  <si>
+    <t>Liam</t>
+  </si>
+  <si>
+    <t>Ava</t>
+  </si>
+  <si>
+    <t>Noah</t>
+  </si>
+  <si>
+    <t>Oliver</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Isabella</t>
+  </si>
+  <si>
+    <t>Elijah</t>
+  </si>
+  <si>
+    <t>Sales Values</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Budget</t>
+  </si>
+  <si>
+    <t>% Change</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>Inkly</t>
+  </si>
+  <si>
+    <t>Kind Ape</t>
+  </si>
+  <si>
+    <t>Pet Feed</t>
+  </si>
+  <si>
+    <t>Right App</t>
+  </si>
+  <si>
+    <t>Mirrrr</t>
+  </si>
+  <si>
+    <t>Halotot</t>
+  </si>
+  <si>
+    <t>Flowrrr</t>
+  </si>
+  <si>
+    <t>Silvrr</t>
+  </si>
+  <si>
+    <t>Starting Price</t>
+  </si>
+  <si>
+    <t>Increase Price by</t>
+  </si>
+  <si>
+    <t>End Price</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,6 +590,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -526,7 +630,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -663,15 +767,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -734,17 +856,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="8">
+    <cellStyle name="Comma 2" xfId="6" xr:uid="{FB7796FF-EE83-4834-81F2-1465ACD8A209}"/>
     <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{DA3F0C31-CC79-4E87-AFB1-7A6099006D56}"/>
     <cellStyle name="Hyperlink 3" xfId="4" xr:uid="{C4CE5DF7-4AB3-4E3B-B8AF-6BB298E76A64}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{27E0D15E-1D11-4E0E-9819-2BF1029C6403}"/>
+    <cellStyle name="Normal 3" xfId="5" xr:uid="{323CA2F9-9C7C-4081-B581-9FDBBADDCB50}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent 2" xfId="7" xr:uid="{E8494675-2B61-4121-80E1-BBCDC14FBEE3}"/>
   </cellStyles>
   <dxfs count="28">
     <dxf>
@@ -1622,19 +1762,19 @@
         <v>5</v>
       </c>
       <c r="J4" s="8">
-        <f>B4/$F4</f>
+        <f t="shared" ref="J4:M6" si="0">B4/$F4</f>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="K4" s="8">
-        <f>C4/$F4</f>
+        <f t="shared" si="0"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="L4" s="8">
-        <f>D4/$F4</f>
+        <f t="shared" si="0"/>
         <v>0.45454545454545453</v>
       </c>
       <c r="M4" s="8">
-        <f>E4/$F4</f>
+        <f t="shared" si="0"/>
         <v>0.27272727272727271</v>
       </c>
     </row>
@@ -1655,30 +1795,30 @@
         <v>90</v>
       </c>
       <c r="F5" s="6">
-        <f t="shared" ref="F5:F6" si="0">SUM(B5:E5)</f>
+        <f t="shared" ref="F5:F6" si="1">SUM(B5:E5)</f>
         <v>630</v>
       </c>
       <c r="G5" s="8">
-        <f t="shared" ref="G5:G6" si="1">F5/$F$7</f>
+        <f t="shared" ref="G5:G6" si="2">F5/$F$7</f>
         <v>0.25250501002004005</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="J5" s="8">
-        <f>B5/$F5</f>
+        <f t="shared" si="0"/>
         <v>0.23809523809523808</v>
       </c>
       <c r="K5" s="8">
-        <f>C5/$F5</f>
+        <f t="shared" si="0"/>
         <v>0.3968253968253968</v>
       </c>
       <c r="L5" s="8">
-        <f>D5/$F5</f>
+        <f t="shared" si="0"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="M5" s="8">
-        <f>E5/$F5</f>
+        <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
     </row>
@@ -1699,30 +1839,30 @@
         <v>85</v>
       </c>
       <c r="F6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>765</v>
       </c>
       <c r="G6" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.30661322645290578</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="J6" s="8">
-        <f>B6/$F6</f>
+        <f t="shared" si="0"/>
         <v>0.30065359477124182</v>
       </c>
       <c r="K6" s="8">
-        <f>C6/$F6</f>
+        <f t="shared" si="0"/>
         <v>0.45751633986928103</v>
       </c>
       <c r="L6" s="8">
-        <f>D6/$F6</f>
+        <f t="shared" si="0"/>
         <v>0.13071895424836602</v>
       </c>
       <c r="M6" s="8">
-        <f>E6/$F6</f>
+        <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
     </row>
@@ -1737,17 +1877,17 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
@@ -4322,17 +4462,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A141A2CA-4D73-477C-AC13-C10AC1812F6A}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="38"/>
+      <c r="B1" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4346,4 +4486,440 @@
     <oddFooter>&amp;L&amp;"-,Bold"AKSHAY PAUNIKAR&amp;RPage &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32DE359B-B384-418D-A5CC-5046733A215D}">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5:P8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15" thickBot="1">
+      <c r="A1" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="B3" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="B4" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="41">
+        <v>480</v>
+      </c>
+      <c r="D4" s="41">
+        <v>500</v>
+      </c>
+      <c r="E4" s="43">
+        <f>C4/D4</f>
+        <v>0.96</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="I4" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="J4" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="K4" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="N4" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="O4" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="P4" s="41" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="B5" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="41">
+        <v>470</v>
+      </c>
+      <c r="D5" s="41">
+        <v>500</v>
+      </c>
+      <c r="E5" s="43">
+        <f t="shared" ref="E5:E13" si="0">C5/D5</f>
+        <v>0.94</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="41">
+        <v>14432</v>
+      </c>
+      <c r="J5" s="41">
+        <v>15113</v>
+      </c>
+      <c r="K5" s="43">
+        <f>I5/J5-1</f>
+        <v>-4.5060543902600392E-2</v>
+      </c>
+      <c r="N5" s="41">
+        <v>100</v>
+      </c>
+      <c r="O5" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="P5" s="41">
+        <f>N5*(1+O5)</f>
+        <v>110.00000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="B6" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="41">
+        <v>468</v>
+      </c>
+      <c r="D6" s="41">
+        <v>500</v>
+      </c>
+      <c r="E6" s="43">
+        <f t="shared" si="0"/>
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="41">
+        <v>17990</v>
+      </c>
+      <c r="J6" s="41">
+        <v>18181</v>
+      </c>
+      <c r="K6" s="43">
+        <f t="shared" ref="K6:K16" si="1">I6/J6-1</f>
+        <v>-1.0505472746273559E-2</v>
+      </c>
+      <c r="N6" s="41">
+        <v>50</v>
+      </c>
+      <c r="O6" s="43">
+        <v>-0.2</v>
+      </c>
+      <c r="P6" s="41">
+        <f t="shared" ref="P6:P8" si="2">N6*(1+O6)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="B7" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="41">
+        <v>423</v>
+      </c>
+      <c r="D7" s="41">
+        <v>500</v>
+      </c>
+      <c r="E7" s="43">
+        <f t="shared" si="0"/>
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="I7" s="41">
+        <v>15117</v>
+      </c>
+      <c r="J7" s="41">
+        <v>13455</v>
+      </c>
+      <c r="K7" s="43">
+        <f t="shared" si="1"/>
+        <v>0.12352285395763651</v>
+      </c>
+      <c r="N7" s="41">
+        <v>80</v>
+      </c>
+      <c r="O7" s="43">
+        <v>0.05</v>
+      </c>
+      <c r="P7" s="41">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="B8" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="41">
+        <v>415</v>
+      </c>
+      <c r="D8" s="41">
+        <v>500</v>
+      </c>
+      <c r="E8" s="43">
+        <f t="shared" si="0"/>
+        <v>0.83</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="41">
+        <v>11154</v>
+      </c>
+      <c r="J8" s="41">
+        <v>12031</v>
+      </c>
+      <c r="K8" s="43">
+        <f t="shared" si="1"/>
+        <v>-7.2895021195245602E-2</v>
+      </c>
+      <c r="N8" s="41">
+        <v>20</v>
+      </c>
+      <c r="O8" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="P8" s="41">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="B9" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="41">
+        <v>406</v>
+      </c>
+      <c r="D9" s="41">
+        <v>500</v>
+      </c>
+      <c r="E9" s="43">
+        <f t="shared" si="0"/>
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="41">
+        <v>11022</v>
+      </c>
+      <c r="J9" s="41">
+        <v>14600</v>
+      </c>
+      <c r="K9" s="43">
+        <f t="shared" si="1"/>
+        <v>-0.24506849315068491</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="B10" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="41">
+        <v>358</v>
+      </c>
+      <c r="D10" s="41">
+        <v>500</v>
+      </c>
+      <c r="E10" s="43">
+        <f t="shared" si="0"/>
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="H10" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="I10" s="41">
+        <v>8905</v>
+      </c>
+      <c r="J10" s="41">
+        <v>9096</v>
+      </c>
+      <c r="K10" s="43">
+        <f t="shared" si="1"/>
+        <v>-2.0998240985048322E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="B11" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="41">
+        <v>369</v>
+      </c>
+      <c r="D11" s="41">
+        <v>500</v>
+      </c>
+      <c r="E11" s="43">
+        <f t="shared" si="0"/>
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="I11" s="41">
+        <v>16735</v>
+      </c>
+      <c r="J11" s="41">
+        <v>18207</v>
+      </c>
+      <c r="K11" s="43">
+        <f t="shared" si="1"/>
+        <v>-8.0848025484703712E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="B12" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="41">
+        <v>358</v>
+      </c>
+      <c r="D12" s="41">
+        <v>500</v>
+      </c>
+      <c r="E12" s="43">
+        <f t="shared" si="0"/>
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I12" s="41">
+        <v>3635</v>
+      </c>
+      <c r="J12" s="41">
+        <v>3579</v>
+      </c>
+      <c r="K12" s="43">
+        <f t="shared" si="1"/>
+        <v>1.5646828723107076E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="B13" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="41">
+        <v>320</v>
+      </c>
+      <c r="D13" s="41">
+        <v>500</v>
+      </c>
+      <c r="E13" s="43">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="I13" s="41">
+        <v>15627</v>
+      </c>
+      <c r="J13" s="41">
+        <v>14634</v>
+      </c>
+      <c r="K13" s="43">
+        <f t="shared" si="1"/>
+        <v>6.7855678556785648E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="H14" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="I14" s="41">
+        <v>7270</v>
+      </c>
+      <c r="J14" s="41">
+        <v>7158</v>
+      </c>
+      <c r="K14" s="43">
+        <f t="shared" si="1"/>
+        <v>1.5646828723107076E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="H15" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="I15" s="41">
+        <v>5955</v>
+      </c>
+      <c r="J15" s="41">
+        <v>5977</v>
+      </c>
+      <c r="K15" s="43">
+        <f t="shared" si="1"/>
+        <v>-3.6807763091851742E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="H16" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I16" s="41">
+        <v>7666</v>
+      </c>
+      <c r="J16" s="41">
+        <v>7099</v>
+      </c>
+      <c r="K16" s="43">
+        <f t="shared" si="1"/>
+        <v>7.9870404282293306E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Two methods to change CASE of textual data
</commit_message>
<xml_diff>
--- a/Microsoft_Excel_by_Leila_Gharani.xlsx
+++ b/Microsoft_Excel_by_Leila_Gharani.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iNeuron\Microsoft_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF09668-3EEF-4845-AA18-3FAEF7EAA26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DC7F75-298B-4522-A524-6600322AEEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day-1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Day-8" sheetId="10" r:id="rId8"/>
     <sheet name="Day-9" sheetId="11" r:id="rId9"/>
     <sheet name="Day-10" sheetId="12" r:id="rId10"/>
+    <sheet name="Day-11" sheetId="13" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Day-2'!$C$3:$F$29</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="169">
   <si>
     <t>Absolute, Relative and Mixed Cell Referencing</t>
   </si>
@@ -532,6 +533,72 @@
   </si>
   <si>
     <t>Let's say that you want to edit a formula so if you are in point model and use arrow keys it will move to the next cells. Edit mode allows you to edit the formula or text.</t>
+  </si>
+  <si>
+    <t>CASE of Text Data</t>
+  </si>
+  <si>
+    <t>#1 Formula Method</t>
+  </si>
+  <si>
+    <t>Upper Case</t>
+  </si>
+  <si>
+    <t>Lower Case</t>
+  </si>
+  <si>
+    <t>Proper Case</t>
+  </si>
+  <si>
+    <t>Gary Miller</t>
+  </si>
+  <si>
+    <t>Gary   miller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virat koHlI  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  SaCHiN   TenDULkAr  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RiChaRD   FeYNmaNN  </t>
+  </si>
+  <si>
+    <t>#2 Flash Fill Method</t>
+  </si>
+  <si>
+    <t>GARY MILLER</t>
+  </si>
+  <si>
+    <t>VIRAT KOHLI</t>
+  </si>
+  <si>
+    <t>SACHIN TENDULKAR</t>
+  </si>
+  <si>
+    <t>RICHARD FEYNMANN</t>
+  </si>
+  <si>
+    <t>gary miller</t>
+  </si>
+  <si>
+    <t>virat kohli</t>
+  </si>
+  <si>
+    <t>sachin tendulkar</t>
+  </si>
+  <si>
+    <t>richard feynmann</t>
+  </si>
+  <si>
+    <t>Virat Kohli</t>
+  </si>
+  <si>
+    <t>Sachin Tendulkar</t>
+  </si>
+  <si>
+    <t>Richard Feynmann</t>
   </si>
 </sst>
 </file>
@@ -908,6 +975,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -921,8 +989,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma 2" xfId="6" xr:uid="{FB7796FF-EE83-4834-81F2-1465ACD8A209}"/>
@@ -1727,7 +1794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B23" sqref="B23:D24"/>
     </sheetView>
   </sheetViews>
@@ -1740,13 +1807,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="3"/>
@@ -1925,17 +1992,17 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
@@ -1948,37 +2015,36 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="42" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="47" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="42" t="s">
         <v>139</v>
       </c>
       <c r="B18" t="s">
         <v>143</v>
       </c>
-      <c r="K18" s="48"/>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="47" t="s">
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="42" t="s">
         <v>140</v>
       </c>
       <c r="B19" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="47" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="42" t="s">
         <v>141</v>
       </c>
       <c r="B20" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="47" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="42" t="s">
         <v>142</v>
       </c>
       <c r="B21" t="s">
@@ -2000,7 +2066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FD6CB2-93D0-4DD1-99B9-B44D93E8E056}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -2013,10 +2079,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="44"/>
+      <c r="B1" s="45"/>
     </row>
     <row r="3" spans="1:6">
       <c r="C3" s="40" t="s">
@@ -2511,6 +2577,202 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AC54C2-672F-4185-AAA6-F9DC37923135}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1">
+      <c r="A1" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="43"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1">
+      <c r="A3" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="43"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1">
+      <c r="C4" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="C5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" t="str">
+        <f>TRIM(UPPER(C5))</f>
+        <v>GARY MILLER</v>
+      </c>
+      <c r="E5" t="str">
+        <f>TRIM(LOWER(C5))</f>
+        <v>gary miller</v>
+      </c>
+      <c r="F5" t="str">
+        <f>TRIM(PROPER(C5))</f>
+        <v>Gary Miller</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="C6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" ref="D6:D8" si="0">TRIM(UPPER(C6))</f>
+        <v>VIRAT KOHLI</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" ref="E6:E8" si="1">TRIM(LOWER(C6))</f>
+        <v>virat kohli</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:F8" si="2">TRIM(PROPER(C6))</f>
+        <v>Virat Kohli</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="C7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>SACHIN TENDULKAR</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>sachin tendulkar</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="2"/>
+        <v>Sachin Tendulkar</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="C8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>RICHARD FEYNMANN</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>richard feynmann</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="2"/>
+        <v>Richard Feynmann</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1">
+      <c r="A10" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="43"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1">
+      <c r="C11" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" s="48" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="C12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" t="s">
+        <v>162</v>
+      </c>
+      <c r="F12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="C13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" t="s">
+        <v>159</v>
+      </c>
+      <c r="E13" t="s">
+        <v>163</v>
+      </c>
+      <c r="F13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="C14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="C15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E15" t="s">
+        <v>165</v>
+      </c>
+      <c r="F15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2533,10 +2795,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="42"/>
+      <c r="B1" s="43"/>
       <c r="D1" t="s">
         <v>26</v>
       </c>
@@ -2964,11 +3226,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
       <c r="I1" s="30" t="s">
         <v>14</v>
       </c>
@@ -3447,10 +3709,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="42"/>
+      <c r="B1" s="43"/>
     </row>
     <row r="4" spans="1:6">
       <c r="C4" s="31" t="s">
@@ -3983,10 +4245,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="42"/>
+      <c r="B1" s="43"/>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" t="s">
@@ -4614,11 +4876,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -4867,11 +5129,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
@@ -5075,10 +5337,10 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="44"/>
+      <c r="B1" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5119,14 +5381,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" thickBot="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
     </row>
     <row r="3" spans="1:16">
       <c r="B3" s="37" t="s">
@@ -5141,12 +5403,12 @@
       <c r="E3" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="47" t="s">
         <v>120</v>
       </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
     </row>
     <row r="4" spans="1:16">
       <c r="B4" s="38" t="s">

</xml_diff>

<commit_message>
Lock Cells & Protect Excel Worksheet
</commit_message>
<xml_diff>
--- a/Microsoft_Excel_by_Leila_Gharani.xlsx
+++ b/Microsoft_Excel_by_Leila_Gharani.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iNeuron\Microsoft_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DC7F75-298B-4522-A524-6600322AEEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC979E5F-75D8-4F67-A9F0-E9576EFB015A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day-1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Day-9" sheetId="11" r:id="rId9"/>
     <sheet name="Day-10" sheetId="12" r:id="rId10"/>
     <sheet name="Day-11" sheetId="13" r:id="rId11"/>
+    <sheet name="Day-12" sheetId="14" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Day-2'!$C$3:$F$29</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="214">
   <si>
     <t>Absolute, Relative and Mixed Cell Referencing</t>
   </si>
@@ -599,6 +600,141 @@
   </si>
   <si>
     <t>Richard Feynmann</t>
+  </si>
+  <si>
+    <t>Lock Cells &amp; Protect Excel Worksheet</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Phase 1</t>
+  </si>
+  <si>
+    <t>Phase 2</t>
+  </si>
+  <si>
+    <t>Phase 3</t>
+  </si>
+  <si>
+    <t>Phase 4</t>
+  </si>
+  <si>
+    <t>Phase 5</t>
+  </si>
+  <si>
+    <t>Phase 6</t>
+  </si>
+  <si>
+    <t>Phase 7</t>
+  </si>
+  <si>
+    <t>Phase 8</t>
+  </si>
+  <si>
+    <t>Phase 9</t>
+  </si>
+  <si>
+    <t>Phase 10</t>
+  </si>
+  <si>
+    <t>Phase 11</t>
+  </si>
+  <si>
+    <t>Phase 12</t>
+  </si>
+  <si>
+    <t>Phase 13</t>
+  </si>
+  <si>
+    <t>Phase 14</t>
+  </si>
+  <si>
+    <t>Phase 15</t>
+  </si>
+  <si>
+    <t>Phase 16</t>
+  </si>
+  <si>
+    <t>Phase 17</t>
+  </si>
+  <si>
+    <t>Phase 18</t>
+  </si>
+  <si>
+    <t>Phase 19</t>
+  </si>
+  <si>
+    <t>Phase 20</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
@@ -728,7 +864,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -889,6 +1025,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -900,7 +1056,7 @@
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -979,6 +1135,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -989,7 +1149,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma 2" xfId="6" xr:uid="{FB7796FF-EE83-4834-81F2-1465ACD8A209}"/>
@@ -1807,13 +1979,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="3"/>
@@ -1992,17 +2164,17 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
@@ -2079,10 +2251,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="45"/>
+      <c r="B1" s="47"/>
     </row>
     <row r="3" spans="1:6">
       <c r="C3" s="40" t="s">
@@ -2586,7 +2758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AC54C2-672F-4185-AAA6-F9DC37923135}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -2599,28 +2771,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="45"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="43"/>
+      <c r="B3" s="45"/>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1">
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="44" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2693,22 +2865,22 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="B10" s="43"/>
+      <c r="B10" s="45"/>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1">
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="F11" s="48" t="s">
+      <c r="F11" s="44" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2774,6 +2946,395 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A10:B10"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C131DAA7-CAAB-4145-A204-2395D99BDB4A}">
+  <dimension ref="A1:U13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="15" thickBot="1">
+      <c r="A1" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" thickBot="1">
+      <c r="A3" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="H3" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="I3" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="J3" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="K3" s="43" t="s">
+        <v>180</v>
+      </c>
+      <c r="L3" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="M3" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="N3" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="O3" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="P3" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q3" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="R3" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="S3" s="43" t="s">
+        <v>188</v>
+      </c>
+      <c r="T3" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="U3" s="43" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="51">
+        <v>1</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="52" t="s">
+        <v>192</v>
+      </c>
+      <c r="M4" s="53"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="53"/>
+      <c r="R4" s="53"/>
+      <c r="S4" s="53"/>
+      <c r="T4" s="53"/>
+      <c r="U4" s="53"/>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" s="51">
+        <v>2</v>
+      </c>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="52" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="53"/>
+      <c r="T5" s="53"/>
+      <c r="U5" s="52" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="51">
+        <v>3</v>
+      </c>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="52" t="s">
+        <v>195</v>
+      </c>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="52" t="s">
+        <v>196</v>
+      </c>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="53"/>
+      <c r="Q6" s="53"/>
+      <c r="R6" s="53"/>
+      <c r="S6" s="52" t="s">
+        <v>197</v>
+      </c>
+      <c r="T6" s="53"/>
+      <c r="U6" s="53"/>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="51">
+        <v>4</v>
+      </c>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="52" t="s">
+        <v>198</v>
+      </c>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="52" t="s">
+        <v>199</v>
+      </c>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="53"/>
+      <c r="Q7" s="52" t="s">
+        <v>200</v>
+      </c>
+      <c r="R7" s="53"/>
+      <c r="S7" s="53"/>
+      <c r="T7" s="53"/>
+      <c r="U7" s="53"/>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="51">
+        <v>5</v>
+      </c>
+      <c r="B8" s="53"/>
+      <c r="C8" s="52" t="s">
+        <v>201</v>
+      </c>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="52" t="s">
+        <v>202</v>
+      </c>
+      <c r="O8" s="53"/>
+      <c r="P8" s="53"/>
+      <c r="Q8" s="53"/>
+      <c r="R8" s="52" t="s">
+        <v>203</v>
+      </c>
+      <c r="S8" s="53"/>
+      <c r="T8" s="53"/>
+      <c r="U8" s="53"/>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="51">
+        <v>6</v>
+      </c>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="52" t="s">
+        <v>204</v>
+      </c>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="52" t="s">
+        <v>205</v>
+      </c>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="53"/>
+      <c r="O9" s="53"/>
+      <c r="P9" s="53"/>
+      <c r="Q9" s="53"/>
+      <c r="R9" s="53"/>
+      <c r="S9" s="53"/>
+      <c r="T9" s="53"/>
+      <c r="U9" s="53"/>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="51">
+        <v>7</v>
+      </c>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="53"/>
+      <c r="O10" s="53"/>
+      <c r="P10" s="53"/>
+      <c r="Q10" s="53"/>
+      <c r="R10" s="53"/>
+      <c r="S10" s="53"/>
+      <c r="T10" s="53"/>
+      <c r="U10" s="53"/>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="51">
+        <v>8</v>
+      </c>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="52" t="s">
+        <v>206</v>
+      </c>
+      <c r="K11" s="53"/>
+      <c r="L11" s="52" t="s">
+        <v>207</v>
+      </c>
+      <c r="M11" s="53"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="53"/>
+      <c r="P11" s="53"/>
+      <c r="Q11" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="R11" s="53"/>
+      <c r="S11" s="53"/>
+      <c r="T11" s="53"/>
+      <c r="U11" s="52" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="51">
+        <v>9</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="52" t="s">
+        <v>211</v>
+      </c>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="52" t="s">
+        <v>212</v>
+      </c>
+      <c r="O12" s="53"/>
+      <c r="P12" s="53"/>
+      <c r="Q12" s="53"/>
+      <c r="R12" s="53"/>
+      <c r="S12" s="53"/>
+      <c r="T12" s="53"/>
+      <c r="U12" s="53"/>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="51">
+        <v>10</v>
+      </c>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="52" t="s">
+        <v>213</v>
+      </c>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="53"/>
+      <c r="O13" s="53"/>
+      <c r="P13" s="53"/>
+      <c r="Q13" s="53"/>
+      <c r="R13" s="53"/>
+      <c r="S13" s="53"/>
+      <c r="T13" s="53"/>
+      <c r="U13" s="53"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2795,10 +3356,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="45"/>
       <c r="D1" t="s">
         <v>26</v>
       </c>
@@ -3226,11 +3787,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
       <c r="I1" s="30" t="s">
         <v>14</v>
       </c>
@@ -3709,10 +4270,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="45"/>
     </row>
     <row r="4" spans="1:6">
       <c r="C4" s="31" t="s">
@@ -4245,10 +4806,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="45"/>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" t="s">
@@ -4876,11 +5437,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -5129,11 +5690,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
@@ -5337,10 +5898,10 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="45"/>
+      <c r="B1" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5381,14 +5942,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" thickBot="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
     </row>
     <row r="3" spans="1:16">
       <c r="B3" s="37" t="s">
@@ -5403,12 +5964,12 @@
       <c r="E3" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
     </row>
     <row r="4" spans="1:16">
       <c r="B4" s="38" t="s">

</xml_diff>

<commit_message>
Add Test to Beginning or End of Values
</commit_message>
<xml_diff>
--- a/Microsoft_Excel_by_Leila_Gharani.xlsx
+++ b/Microsoft_Excel_by_Leila_Gharani.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iNeuron\Microsoft_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AC1989-8180-4071-B593-6B69830BFE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43ADE86-5593-4033-9FC3-0E29B9470C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day-1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="Day-12" sheetId="14" r:id="rId12"/>
     <sheet name="Day-13" sheetId="15" r:id="rId13"/>
     <sheet name="Day-14" sheetId="16" r:id="rId14"/>
+    <sheet name="Day-15" sheetId="17" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Day-14'!$F$3:$F$11</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="319">
   <si>
     <t>Absolute, Relative and Mixed Cell Referencing</t>
   </si>
@@ -983,13 +984,88 @@
   <si>
     <t>Finance Average Salary</t>
   </si>
+  <si>
+    <t>Add Text to Beginning or End of Values</t>
+  </si>
+  <si>
+    <t>#1 Flash Fill</t>
+  </si>
+  <si>
+    <t>ID 270</t>
+  </si>
+  <si>
+    <t>ID 450</t>
+  </si>
+  <si>
+    <t>ID 781</t>
+  </si>
+  <si>
+    <t>ID 562</t>
+  </si>
+  <si>
+    <t>ID 124</t>
+  </si>
+  <si>
+    <t>ID 892</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Luna</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>Leena</t>
+  </si>
+  <si>
+    <t>Arthur</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>ID-Tom</t>
+  </si>
+  <si>
+    <t>ID-Luna</t>
+  </si>
+  <si>
+    <t>ID-Sara</t>
+  </si>
+  <si>
+    <t>ID-Leena</t>
+  </si>
+  <si>
+    <t>ID-Arthur</t>
+  </si>
+  <si>
+    <t>ID-James</t>
+  </si>
+  <si>
+    <t>#2 Formula</t>
+  </si>
+  <si>
+    <t>Leila</t>
+  </si>
+  <si>
+    <t>#3 Custom Format</t>
+  </si>
+  <si>
+    <t>"#" - Numbers, "@" - Text</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="&quot;ID &quot;#"/>
+    <numFmt numFmtId="167" formatCode="&quot;ID &quot;@"/>
+    <numFmt numFmtId="169" formatCode="&quot;ID &quot;#;;;&quot;ID &quot;@"/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -1336,7 +1412,7 @@
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1432,6 +1508,10 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1451,10 +1531,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Comma 2" xfId="6" xr:uid="{FB7796FF-EE83-4834-81F2-1465ACD8A209}"/>
@@ -2467,13 +2546,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="3"/>
@@ -2652,17 +2731,17 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
@@ -2739,10 +2818,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="58"/>
     </row>
     <row r="3" spans="1:6">
       <c r="C3" s="40" t="s">
@@ -3259,16 +3338,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="56"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="52"/>
+      <c r="B3" s="56"/>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1">
       <c r="C4" s="44" t="s">
@@ -3353,10 +3432,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="B10" s="52"/>
+      <c r="B10" s="56"/>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1">
       <c r="C11" s="44" t="s">
@@ -3449,12 +3528,12 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:21" ht="15" thickBot="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="56" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1">
       <c r="A3" s="45" t="s">
@@ -3864,11 +3943,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.399999999999999">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="62" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
       <c r="D1" s="48"/>
       <c r="E1" s="48"/>
       <c r="F1" s="48"/>
@@ -3891,10 +3970,10 @@
       <c r="E3" s="51" t="s">
         <v>218</v>
       </c>
-      <c r="I3" s="57" t="s">
+      <c r="I3" s="61" t="s">
         <v>219</v>
       </c>
-      <c r="J3" s="57"/>
+      <c r="J3" s="61"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="9" t="s">
@@ -4859,7 +4938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CA4F55-CAD1-49F7-A8EB-DD8BF5EC43C9}">
   <dimension ref="B1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -4872,37 +4951,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1">
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="56" t="s">
         <v>276</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="3" spans="2:9" ht="15" thickBot="1">
-      <c r="E3" s="62" t="s">
+      <c r="E3" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="62" t="s">
+      <c r="F3" s="55" t="s">
         <v>277</v>
       </c>
-      <c r="G3" s="62" t="s">
+      <c r="G3" s="55" t="s">
         <v>278</v>
       </c>
-      <c r="I3" s="62" t="s">
+      <c r="I3" s="55" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="4" spans="2:9">
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="53" t="s">
         <v>152</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="53" t="s">
         <v>286</v>
       </c>
-      <c r="G4" s="61">
+      <c r="G4" s="54">
         <v>60270</v>
       </c>
-      <c r="I4" s="60" t="s">
+      <c r="I4" s="53" t="s">
         <v>286</v>
       </c>
     </row>
@@ -4913,7 +4992,7 @@
       <c r="F5" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="G5" s="59">
+      <c r="G5" s="52">
         <v>39627</v>
       </c>
       <c r="I5" s="9" t="s">
@@ -4927,7 +5006,7 @@
       <c r="F6" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="G6" s="59">
+      <c r="G6" s="52">
         <v>29727</v>
       </c>
       <c r="I6" s="9" t="s">
@@ -4941,7 +5020,7 @@
       <c r="F7" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="G7" s="59">
+      <c r="G7" s="52">
         <v>93668</v>
       </c>
     </row>
@@ -4952,7 +5031,7 @@
       <c r="F8" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="G8" s="59">
+      <c r="G8" s="52">
         <v>134000</v>
       </c>
     </row>
@@ -4963,7 +5042,7 @@
       <c r="F9" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="G9" s="59">
+      <c r="G9" s="52">
         <v>34808</v>
       </c>
     </row>
@@ -4974,7 +5053,7 @@
       <c r="F10" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="G10" s="59">
+      <c r="G10" s="52">
         <v>134468</v>
       </c>
     </row>
@@ -4985,7 +5064,7 @@
       <c r="F11" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="G11" s="59">
+      <c r="G11" s="52">
         <v>45000</v>
       </c>
     </row>
@@ -5055,6 +5134,345 @@
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5D0DC5-F573-4A8A-87A3-3DC461D5D3A2}">
+  <dimension ref="A1:I41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1">
+      <c r="A1" s="56" t="s">
+        <v>295</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1">
+      <c r="A3" s="56" t="s">
+        <v>296</v>
+      </c>
+      <c r="B3" s="56"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5">
+        <v>270</v>
+      </c>
+      <c r="D5" t="s">
+        <v>297</v>
+      </c>
+      <c r="F5" t="s">
+        <v>303</v>
+      </c>
+      <c r="G5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="C6">
+        <v>450</v>
+      </c>
+      <c r="D6" t="s">
+        <v>298</v>
+      </c>
+      <c r="F6" t="s">
+        <v>304</v>
+      </c>
+      <c r="G6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7">
+        <v>781</v>
+      </c>
+      <c r="D7" t="s">
+        <v>299</v>
+      </c>
+      <c r="F7" t="s">
+        <v>305</v>
+      </c>
+      <c r="G7" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="C8">
+        <v>562</v>
+      </c>
+      <c r="D8" t="s">
+        <v>300</v>
+      </c>
+      <c r="F8" t="s">
+        <v>306</v>
+      </c>
+      <c r="G8" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="C9">
+        <v>124</v>
+      </c>
+      <c r="D9" t="s">
+        <v>301</v>
+      </c>
+      <c r="F9" t="s">
+        <v>307</v>
+      </c>
+      <c r="G9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="C10">
+        <v>892</v>
+      </c>
+      <c r="D10" t="s">
+        <v>302</v>
+      </c>
+      <c r="F10" t="s">
+        <v>308</v>
+      </c>
+      <c r="G10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" thickBot="1">
+      <c r="A12" s="56" t="s">
+        <v>315</v>
+      </c>
+      <c r="B12" s="56"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="C14">
+        <v>270</v>
+      </c>
+      <c r="D14" t="str">
+        <f>"ID "&amp;C14</f>
+        <v>ID 270</v>
+      </c>
+      <c r="F14" t="s">
+        <v>303</v>
+      </c>
+      <c r="G14" t="str">
+        <f>"ID-"&amp;F14&amp;" Sales"</f>
+        <v>ID-Tom Sales</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="C15">
+        <v>450</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" ref="D15:D19" si="0">"ID "&amp;C15</f>
+        <v>ID 450</v>
+      </c>
+      <c r="F15" t="s">
+        <v>304</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" ref="G15:G19" si="1">"ID-"&amp;F15&amp;" Sales"</f>
+        <v>ID-Luna Sales</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="C16">
+        <v>781</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>ID 781</v>
+      </c>
+      <c r="F16" t="s">
+        <v>305</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>ID-Sara Sales</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="C17">
+        <v>562</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>ID 562</v>
+      </c>
+      <c r="F17" t="s">
+        <v>306</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v>ID-Leena Sales</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="C18">
+        <v>124</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>ID 124</v>
+      </c>
+      <c r="F18" t="s">
+        <v>307</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v>ID-Arthur Sales</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="C19">
+        <v>892</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>ID 892</v>
+      </c>
+      <c r="F19" t="s">
+        <v>316</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v>ID-Leila Sales</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" thickBot="1">
+      <c r="A21" s="56" t="s">
+        <v>317</v>
+      </c>
+      <c r="B21" s="56"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="C23" s="63">
+        <v>270</v>
+      </c>
+      <c r="F23" s="64" t="s">
+        <v>303</v>
+      </c>
+      <c r="I23" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="C24" s="63">
+        <v>450</v>
+      </c>
+      <c r="F24" s="64" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="C25" s="63">
+        <v>781</v>
+      </c>
+      <c r="F25" s="64" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="C26" s="63">
+        <v>562</v>
+      </c>
+      <c r="F26" s="64" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="C27" s="63">
+        <v>124</v>
+      </c>
+      <c r="F27" s="64" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="C28" s="63">
+        <v>892</v>
+      </c>
+      <c r="F28" s="64" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="D30" s="65">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="D31" s="65">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="D32" s="65">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33" s="65">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" s="65">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="D35" s="65">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="D36" s="65" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4">
+      <c r="D37" s="65" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4">
+      <c r="D38" s="65" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4">
+      <c r="D39" s="65" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4">
+      <c r="D40" s="65" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4">
+      <c r="D41" s="65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A21:B21"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5076,10 +5494,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="56"/>
       <c r="D1" t="s">
         <v>26</v>
       </c>
@@ -5507,11 +5925,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
       <c r="I1" s="30" t="s">
         <v>14</v>
       </c>
@@ -5990,10 +6408,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="56"/>
     </row>
     <row r="4" spans="1:6">
       <c r="C4" s="31" t="s">
@@ -6526,10 +6944,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="56"/>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" t="s">
@@ -7157,11 +7575,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -7410,11 +7828,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
@@ -7618,10 +8036,10 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7662,14 +8080,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" thickBot="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
     </row>
     <row r="3" spans="1:16">
       <c r="B3" s="37" t="s">
@@ -7684,12 +8102,12 @@
       <c r="E3" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="H3" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
     </row>
     <row r="4" spans="1:16">
       <c r="B4" s="38" t="s">

</xml_diff>

<commit_message>
Customized Quick Access Toolbar
</commit_message>
<xml_diff>
--- a/Microsoft_Excel_by_Leila_Gharani.xlsx
+++ b/Microsoft_Excel_by_Leila_Gharani.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iNeuron\Microsoft_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43ADE86-5593-4033-9FC3-0E29B9470C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB8A64A-AA1D-468C-8F04-70A2D933BE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day-1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="Day-13" sheetId="15" r:id="rId13"/>
     <sheet name="Day-14" sheetId="16" r:id="rId14"/>
     <sheet name="Day-15" sheetId="17" r:id="rId15"/>
+    <sheet name="Day-16" sheetId="18" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Day-14'!$F$3:$F$11</definedName>
@@ -1063,9 +1064,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="&quot;ID &quot;#"/>
-    <numFmt numFmtId="167" formatCode="&quot;ID &quot;@"/>
-    <numFmt numFmtId="169" formatCode="&quot;ID &quot;#;;;&quot;ID &quot;@"/>
+    <numFmt numFmtId="164" formatCode="&quot;ID &quot;#"/>
+    <numFmt numFmtId="165" formatCode="&quot;ID &quot;@"/>
+    <numFmt numFmtId="166" formatCode="&quot;ID &quot;#;;;&quot;ID &quot;@"/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -1512,6 +1513,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1531,9 +1535,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Comma 2" xfId="6" xr:uid="{FB7796FF-EE83-4834-81F2-1465ACD8A209}"/>
@@ -2546,13 +2547,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="3"/>
@@ -2731,17 +2732,17 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
@@ -2818,10 +2819,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="58"/>
+      <c r="B1" s="61"/>
     </row>
     <row r="3" spans="1:6">
       <c r="C3" s="40" t="s">
@@ -3338,16 +3339,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="59" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="56"/>
+      <c r="B1" s="59"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="56"/>
+      <c r="B3" s="59"/>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1">
       <c r="C4" s="44" t="s">
@@ -3432,10 +3433,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="B10" s="56"/>
+      <c r="B10" s="59"/>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1">
       <c r="C11" s="44" t="s">
@@ -3528,12 +3529,12 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:21" ht="15" thickBot="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="59" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1">
       <c r="A3" s="45" t="s">
@@ -3943,11 +3944,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.399999999999999">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="65" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
       <c r="D1" s="48"/>
       <c r="E1" s="48"/>
       <c r="F1" s="48"/>
@@ -3970,10 +3971,10 @@
       <c r="E3" s="51" t="s">
         <v>218</v>
       </c>
-      <c r="I3" s="61" t="s">
+      <c r="I3" s="64" t="s">
         <v>219</v>
       </c>
-      <c r="J3" s="61"/>
+      <c r="J3" s="64"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="9" t="s">
@@ -4951,11 +4952,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="59" t="s">
         <v>276</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
     </row>
     <row r="3" spans="2:9" ht="15" thickBot="1">
       <c r="E3" s="55" t="s">
@@ -5142,25 +5143,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5D0DC5-F573-4A8A-87A3-3DC461D5D3A2}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="59" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="59" t="s">
         <v>296</v>
       </c>
-      <c r="B3" s="56"/>
+      <c r="B3" s="59"/>
     </row>
     <row r="5" spans="1:7">
       <c r="C5">
@@ -5247,10 +5248,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="59" t="s">
         <v>315</v>
       </c>
-      <c r="B12" s="56"/>
+      <c r="B12" s="59"/>
     </row>
     <row r="14" spans="1:7">
       <c r="C14">
@@ -5349,16 +5350,16 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1">
-      <c r="A21" s="56" t="s">
+      <c r="A21" s="59" t="s">
         <v>317</v>
       </c>
-      <c r="B21" s="56"/>
+      <c r="B21" s="59"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="C23" s="63">
+      <c r="C23" s="56">
         <v>270</v>
       </c>
-      <c r="F23" s="64" t="s">
+      <c r="F23" s="57" t="s">
         <v>303</v>
       </c>
       <c r="I23" t="s">
@@ -5366,102 +5367,102 @@
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="C24" s="63">
+      <c r="C24" s="56">
         <v>450</v>
       </c>
-      <c r="F24" s="64" t="s">
+      <c r="F24" s="57" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="C25" s="63">
+      <c r="C25" s="56">
         <v>781</v>
       </c>
-      <c r="F25" s="64" t="s">
+      <c r="F25" s="57" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="C26" s="63">
+      <c r="C26" s="56">
         <v>562</v>
       </c>
-      <c r="F26" s="64" t="s">
+      <c r="F26" s="57" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="C27" s="63">
+      <c r="C27" s="56">
         <v>124</v>
       </c>
-      <c r="F27" s="64" t="s">
+      <c r="F27" s="57" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="C28" s="63">
+      <c r="C28" s="56">
         <v>892</v>
       </c>
-      <c r="F28" s="64" t="s">
+      <c r="F28" s="57" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="D30" s="65">
+      <c r="D30" s="58">
         <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="D31" s="65">
+      <c r="D31" s="58">
         <v>450</v>
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="D32" s="65">
+      <c r="D32" s="58">
         <v>781</v>
       </c>
     </row>
     <row r="33" spans="4:4">
-      <c r="D33" s="65">
+      <c r="D33" s="58">
         <v>562</v>
       </c>
     </row>
     <row r="34" spans="4:4">
-      <c r="D34" s="65">
+      <c r="D34" s="58">
         <v>124</v>
       </c>
     </row>
     <row r="35" spans="4:4">
-      <c r="D35" s="65">
+      <c r="D35" s="58">
         <v>892</v>
       </c>
     </row>
     <row r="36" spans="4:4">
-      <c r="D36" s="65" t="s">
+      <c r="D36" s="58" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="37" spans="4:4">
-      <c r="D37" s="65" t="s">
+      <c r="D37" s="58" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="38" spans="4:4">
-      <c r="D38" s="65" t="s">
+      <c r="D38" s="58" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="39" spans="4:4">
-      <c r="D39" s="65" t="s">
+      <c r="D39" s="58" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="40" spans="4:4">
-      <c r="D40" s="65" t="s">
+      <c r="D40" s="58" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="41" spans="4:4">
-      <c r="D41" s="65" t="s">
+      <c r="D41" s="58" t="s">
         <v>316</v>
       </c>
     </row>
@@ -5473,6 +5474,21 @@
     <mergeCell ref="A21:B21"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11FB7088-5D84-43B7-BE46-C79A60D73A9B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5494,10 +5510,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="56"/>
+      <c r="B1" s="59"/>
       <c r="D1" t="s">
         <v>26</v>
       </c>
@@ -5925,11 +5941,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
       <c r="I1" s="30" t="s">
         <v>14</v>
       </c>
@@ -6408,10 +6424,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="56"/>
+      <c r="B1" s="59"/>
     </row>
     <row r="4" spans="1:6">
       <c r="C4" s="31" t="s">
@@ -6944,10 +6960,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="56"/>
+      <c r="B1" s="59"/>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" t="s">
@@ -7575,11 +7591,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -7828,11 +7844,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
@@ -8036,10 +8052,10 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="58"/>
+      <c r="B1" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8080,14 +8096,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" thickBot="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="3" spans="1:16">
       <c r="B3" s="37" t="s">
@@ -8102,12 +8118,12 @@
       <c r="E3" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="60" t="s">
+      <c r="H3" s="63" t="s">
         <v>120</v>
       </c>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
     </row>
     <row r="4" spans="1:16">
       <c r="B4" s="38" t="s">

</xml_diff>

<commit_message>
Combine Text & Numbers
</commit_message>
<xml_diff>
--- a/Microsoft_Excel_by_Leila_Gharani.xlsx
+++ b/Microsoft_Excel_by_Leila_Gharani.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iNeuron\Microsoft_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB8A64A-AA1D-468C-8F04-70A2D933BE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722DB274-A1F3-4237-BC73-FBEA30BB298D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="327">
   <si>
     <t>Absolute, Relative and Mixed Cell Referencing</t>
   </si>
@@ -1057,16 +1057,42 @@
   <si>
     <t>"#" - Numbers, "@" - Text</t>
   </si>
+  <si>
+    <t>Combine Text &amp; Numbers</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>Jess</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Combine</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;ID &quot;#"/>
     <numFmt numFmtId="165" formatCode="&quot;ID &quot;@"/>
     <numFmt numFmtId="166" formatCode="&quot;ID &quot;#;;;&quot;ID &quot;@"/>
+    <numFmt numFmtId="167" formatCode="&quot;Base: &quot;#,##0"/>
+    <numFmt numFmtId="168" formatCode="&quot;Bonus: &quot;#,##0"/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -1413,7 +1439,7 @@
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1535,6 +1561,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Comma 2" xfId="6" xr:uid="{FB7796FF-EE83-4834-81F2-1465ACD8A209}"/>
@@ -5481,14 +5509,158 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11FB7088-5D84-43B7-BE46-C79A60D73A9B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1">
+      <c r="A1" s="59" t="s">
+        <v>319</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1">
+      <c r="D3" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>320</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" t="s">
+        <v>321</v>
+      </c>
+      <c r="E4">
+        <v>1000</v>
+      </c>
+      <c r="F4" t="str">
+        <f>D4&amp;" $"&amp;TEXT(E4,"#,##0")</f>
+        <v>Bill $1,000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="D5" t="s">
+        <v>322</v>
+      </c>
+      <c r="E5">
+        <v>4000</v>
+      </c>
+      <c r="F5" t="str">
+        <f>D5&amp;" $"&amp;TEXT(E5,"#,##0")</f>
+        <v>Jess $4,000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" t="s">
+        <v>323</v>
+      </c>
+      <c r="E6">
+        <v>2345</v>
+      </c>
+      <c r="F6" t="str">
+        <f>D6&amp;" $"&amp;TEXT(E6,"#,##0")</f>
+        <v>Sarah $2,345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="D7" t="s">
+        <v>324</v>
+      </c>
+      <c r="E7">
+        <v>7890</v>
+      </c>
+      <c r="F7" t="str">
+        <f>D7&amp;" $"&amp;TEXT(E7,"#,##0")</f>
+        <v>Mike $7,890</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" thickBot="1">
+      <c r="D11" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>320</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="D12" t="s">
+        <v>321</v>
+      </c>
+      <c r="E12" s="32">
+        <v>1000</v>
+      </c>
+      <c r="F12">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="D13" t="s">
+        <v>322</v>
+      </c>
+      <c r="E13" s="32">
+        <v>4000</v>
+      </c>
+      <c r="F13">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="D14" t="s">
+        <v>323</v>
+      </c>
+      <c r="E14" s="32">
+        <v>2345</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="D15" t="s">
+        <v>324</v>
+      </c>
+      <c r="E15" s="32">
+        <v>7890</v>
+      </c>
+      <c r="F15">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" thickBot="1">
+      <c r="E16" s="66">
+        <f>SUM(E12:E15)</f>
+        <v>15235</v>
+      </c>
+      <c r="F16" s="67">
+        <f>SUM(F12:F15)</f>
+        <v>1300</v>
+      </c>
+      <c r="G16" s="32">
+        <f>SUM(E16:F16)</f>
+        <v>16535</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Mistakes that we normally do
</commit_message>
<xml_diff>
--- a/Microsoft_Excel_by_Leila_Gharani.xlsx
+++ b/Microsoft_Excel_by_Leila_Gharani.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iNeuron\Microsoft_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722DB274-A1F3-4237-BC73-FBEA30BB298D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFFB66F-648A-4BF0-9E27-7A8FD3767AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day-1" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="Day-14" sheetId="16" r:id="rId14"/>
     <sheet name="Day-15" sheetId="17" r:id="rId15"/>
     <sheet name="Day-16" sheetId="18" r:id="rId16"/>
+    <sheet name="Day-17" sheetId="22" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Day-14'!$F$3:$F$11</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="332">
   <si>
     <t>Absolute, Relative and Mixed Cell Referencing</t>
   </si>
@@ -1080,6 +1081,41 @@
   </si>
   <si>
     <t>Bonus</t>
+  </si>
+  <si>
+    <t>Mistakes that we normally do</t>
+  </si>
+  <si>
+    <t>expand. So, use alignment as Center across selection to avoid this.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>#1 Merging Cells:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> If we have merged cells in between the data that we are analyzing then while performing any calculations, the range will</t>
+    </r>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Total Points</t>
   </si>
 </sst>
 </file>
@@ -1439,7 +1475,7 @@
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1542,6 +1578,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1561,8 +1599,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Comma 2" xfId="6" xr:uid="{FB7796FF-EE83-4834-81F2-1465ACD8A209}"/>
@@ -2575,13 +2614,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="3"/>
@@ -2760,17 +2799,17 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
@@ -2834,7 +2873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FD6CB2-93D0-4DD1-99B9-B44D93E8E056}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A26" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -2847,10 +2886,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="63" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="61"/>
+      <c r="B1" s="63"/>
     </row>
     <row r="3" spans="1:6">
       <c r="C3" s="40" t="s">
@@ -3367,16 +3406,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="59"/>
+      <c r="B1" s="61"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="61" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="59"/>
+      <c r="B3" s="61"/>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1">
       <c r="C4" s="44" t="s">
@@ -3461,10 +3500,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="61" t="s">
         <v>157</v>
       </c>
-      <c r="B10" s="59"/>
+      <c r="B10" s="61"/>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1">
       <c r="C11" s="44" t="s">
@@ -3557,12 +3596,12 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:21" ht="15" thickBot="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1">
       <c r="A3" s="45" t="s">
@@ -3939,7 +3978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ABC3BDE-AAC5-49E8-BABD-DB58712F0EA5}">
   <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
@@ -3972,11 +4011,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.399999999999999">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="67" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
       <c r="D1" s="48"/>
       <c r="E1" s="48"/>
       <c r="F1" s="48"/>
@@ -3999,10 +4038,10 @@
       <c r="E3" s="51" t="s">
         <v>218</v>
       </c>
-      <c r="I3" s="64" t="s">
+      <c r="I3" s="66" t="s">
         <v>219</v>
       </c>
-      <c r="J3" s="64"/>
+      <c r="J3" s="66"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="9" t="s">
@@ -4980,11 +5019,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1">
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="61" t="s">
         <v>276</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
     </row>
     <row r="3" spans="2:9" ht="15" thickBot="1">
       <c r="E3" s="55" t="s">
@@ -5178,18 +5217,18 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="61" t="s">
         <v>296</v>
       </c>
-      <c r="B3" s="59"/>
+      <c r="B3" s="61"/>
     </row>
     <row r="5" spans="1:7">
       <c r="C5">
@@ -5276,10 +5315,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="61" t="s">
         <v>315</v>
       </c>
-      <c r="B12" s="59"/>
+      <c r="B12" s="61"/>
     </row>
     <row r="14" spans="1:7">
       <c r="C14">
@@ -5378,10 +5417,10 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1">
-      <c r="A21" s="59" t="s">
+      <c r="A21" s="61" t="s">
         <v>317</v>
       </c>
-      <c r="B21" s="59"/>
+      <c r="B21" s="61"/>
     </row>
     <row r="23" spans="1:9">
       <c r="C23" s="56">
@@ -5511,8 +5550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11FB7088-5D84-43B7-BE46-C79A60D73A9B}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5523,11 +5562,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>319</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1">
       <c r="D3" s="44" t="s">
@@ -5644,17 +5683,323 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1">
-      <c r="E16" s="66">
+      <c r="E16" s="59">
         <f>SUM(E12:E15)</f>
         <v>15235</v>
       </c>
-      <c r="F16" s="67">
+      <c r="F16" s="60">
         <f>SUM(F12:F15)</f>
         <v>1300</v>
       </c>
       <c r="G16" s="32">
         <f>SUM(E16:F16)</f>
         <v>16535</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28FE2C5E-BB83-4E08-AF3B-F30A2DD5D57E}">
+  <dimension ref="A1:I26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1">
+      <c r="A1" s="61" t="s">
+        <v>327</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="I2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="D3" s="68">
+        <v>2020</v>
+      </c>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="I3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="D4" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="D5" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="38">
+        <v>480</v>
+      </c>
+      <c r="F5" s="38">
+        <v>500</v>
+      </c>
+      <c r="H5" t="s">
+        <v>330</v>
+      </c>
+      <c r="I5">
+        <f>SUM(F5:F26)</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="D6" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="38">
+        <v>470</v>
+      </c>
+      <c r="F6" s="38">
+        <v>500</v>
+      </c>
+      <c r="H6" t="s">
+        <v>331</v>
+      </c>
+      <c r="I6">
+        <f>SUM(E5:E26)</f>
+        <v>8134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="D7" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="38">
+        <v>468</v>
+      </c>
+      <c r="F7" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="D8" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" s="38">
+        <v>423</v>
+      </c>
+      <c r="F8" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="D9" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="38">
+        <v>415</v>
+      </c>
+      <c r="F9" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="D10" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="38">
+        <v>406</v>
+      </c>
+      <c r="F10" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="D11" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" s="38">
+        <v>358</v>
+      </c>
+      <c r="F11" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="D12" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="38">
+        <v>369</v>
+      </c>
+      <c r="F12" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="D13" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" s="38">
+        <v>358</v>
+      </c>
+      <c r="F13" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="D14" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="38">
+        <v>320</v>
+      </c>
+      <c r="F14" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="D15" s="68">
+        <v>2021</v>
+      </c>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="D16" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6">
+      <c r="D17" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="E17" s="38">
+        <v>480</v>
+      </c>
+      <c r="F17" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6">
+      <c r="D18" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="38">
+        <v>470</v>
+      </c>
+      <c r="F18" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6">
+      <c r="D19" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="38">
+        <v>468</v>
+      </c>
+      <c r="F19" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6">
+      <c r="D20" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" s="38">
+        <v>423</v>
+      </c>
+      <c r="F20" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6">
+      <c r="D21" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="38">
+        <v>415</v>
+      </c>
+      <c r="F21" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6">
+      <c r="D22" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="38">
+        <v>406</v>
+      </c>
+      <c r="F22" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6">
+      <c r="D23" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="38">
+        <v>358</v>
+      </c>
+      <c r="F23" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6">
+      <c r="D24" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="38">
+        <v>369</v>
+      </c>
+      <c r="F24" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6">
+      <c r="D25" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" s="38">
+        <v>358</v>
+      </c>
+      <c r="F25" s="38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6">
+      <c r="D26" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="E26" s="38">
+        <v>320</v>
+      </c>
+      <c r="F26" s="38">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -5682,10 +6027,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="59"/>
+      <c r="B1" s="61"/>
       <c r="D1" t="s">
         <v>26</v>
       </c>
@@ -6113,11 +6458,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
       <c r="I1" s="30" t="s">
         <v>14</v>
       </c>
@@ -6596,10 +6941,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="59"/>
+      <c r="B1" s="61"/>
     </row>
     <row r="4" spans="1:6">
       <c r="C4" s="31" t="s">
@@ -7132,10 +7477,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="59"/>
+      <c r="B1" s="61"/>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" t="s">
@@ -7763,11 +8108,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -8016,11 +8361,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
@@ -8224,10 +8569,10 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="61"/>
+      <c r="B1" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8248,7 +8593,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5:P8"/>
+      <selection activeCell="B3" sqref="B3:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8268,14 +8613,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" thickBot="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
     </row>
     <row r="3" spans="1:16">
       <c r="B3" s="37" t="s">
@@ -8290,12 +8635,12 @@
       <c r="E3" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="63" t="s">
+      <c r="H3" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
     </row>
     <row r="4" spans="1:16">
       <c r="B4" s="38" t="s">

</xml_diff>